<commit_message>
TC-61 and TC-62 added
added Create & updated method

verifyTestRunCreation_updationNotificationToast()

in ExecuteLandingPage.Java

added data for TC-61,62
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\executeTestCaseTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BD1538-E7EF-4964-A951-FEE8F1372464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8415972E-7222-48CB-B7B3-C4910DC6ED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="30" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="30" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -50,19 +50,21 @@
     <sheet name="tc050" sheetId="36" r:id="rId35"/>
     <sheet name="tc059" sheetId="45" r:id="rId36"/>
     <sheet name="tc060" sheetId="46" r:id="rId37"/>
-    <sheet name="tc044" sheetId="38" r:id="rId38"/>
-    <sheet name="tc026" sheetId="40" r:id="rId39"/>
-    <sheet name="tc032" sheetId="41" r:id="rId40"/>
-    <sheet name="tc041" sheetId="42" r:id="rId41"/>
-    <sheet name="tc010" sheetId="43" r:id="rId42"/>
-    <sheet name="tc020" sheetId="44" r:id="rId43"/>
+    <sheet name="tc061" sheetId="47" r:id="rId38"/>
+    <sheet name="tc062" sheetId="48" r:id="rId39"/>
+    <sheet name="tc044" sheetId="38" r:id="rId40"/>
+    <sheet name="tc026" sheetId="40" r:id="rId41"/>
+    <sheet name="tc032" sheetId="41" r:id="rId42"/>
+    <sheet name="tc041" sheetId="42" r:id="rId43"/>
+    <sheet name="tc010" sheetId="43" r:id="rId44"/>
+    <sheet name="tc020" sheetId="44" r:id="rId45"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="101">
   <si>
     <t>projectName</t>
   </si>
@@ -2342,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2EC515-C552-4DDF-977F-E873966B2F94}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -2417,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6649F85E-A00A-4D7E-8521-4F9A9E343504}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -2491,88 +2493,142 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="14.5">
-      <c r="A1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.5">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CC7FFB-02DC-44A1-8367-0CF45CAF0BB4}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9B5B1F-8746-4756-94F1-88740BCD638E}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2630,6 +2686,92 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.5">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.5">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2678,7 +2820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2755,7 +2897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2804,7 +2946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>

</xml_diff>